<commit_message>
Added ExcelWriter and ScheduledTasks
</commit_message>
<xml_diff>
--- a/src/main/resources/static/Airports_&_IATA_Codes.xlsx
+++ b/src/main/resources/static/Airports_&_IATA_Codes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Flughafen</t>
   </si>
@@ -36,175 +36,115 @@
     <t>DXB</t>
   </si>
   <si>
+    <t>Hartsfield-Jackson Atlanta International Airport</t>
+  </si>
+  <si>
+    <t>Beijing Capital International Airport</t>
+  </si>
+  <si>
+    <t>Dubai International Airport</t>
+  </si>
+  <si>
+    <t>Los Angeles International Airport</t>
+  </si>
+  <si>
     <t>LAX</t>
   </si>
   <si>
+    <t>Tokyo Haneda International Airport</t>
+  </si>
+  <si>
     <t>HND</t>
   </si>
   <si>
+    <t>O'Hare International Airport</t>
+  </si>
+  <si>
     <t>ORD</t>
   </si>
   <si>
+    <t>London Heathrow Airport</t>
+  </si>
+  <si>
     <t>LHR</t>
   </si>
   <si>
+    <t>Hong Kong International Airport</t>
+  </si>
+  <si>
     <t>HKG</t>
   </si>
   <si>
+    <t>Shanghai Pudong International Airport</t>
+  </si>
+  <si>
     <t>PVG</t>
   </si>
   <si>
+    <t>Aéroport Paris-Charles de Gaulle</t>
+  </si>
+  <si>
     <t>CDG</t>
   </si>
   <si>
+    <t>Amsterdam Airport Schiphol</t>
+  </si>
+  <si>
     <t>AMS</t>
   </si>
   <si>
+    <t>Indira Gandhi International Airport</t>
+  </si>
+  <si>
     <t>DEL</t>
   </si>
   <si>
+    <t>Guangzhou Baiyun International Airport</t>
+  </si>
+  <si>
     <t>CAN</t>
   </si>
   <si>
+    <t>Flughafen Frankfurt am Main</t>
+  </si>
+  <si>
     <t>FRA</t>
   </si>
   <si>
+    <t>Dallas/Fort Worth International Airport</t>
+  </si>
+  <si>
     <t>DFW</t>
   </si>
   <si>
+    <t>Seoul Incheon International Airport</t>
+  </si>
+  <si>
     <t>ICN</t>
   </si>
   <si>
+    <t>Istanbul Atatürk Airport</t>
+  </si>
+  <si>
     <t>IST</t>
   </si>
   <si>
+    <t>Soekarno-Hatta International Airport</t>
+  </si>
+  <si>
     <t>CGK</t>
   </si>
   <si>
+    <t>Singapore Changi Airport</t>
+  </si>
+  <si>
     <t>SIN</t>
   </si>
   <si>
+    <t>Denver International Airport</t>
+  </si>
+  <si>
     <t>DEN</t>
-  </si>
-  <si>
-    <t>BKK</t>
-  </si>
-  <si>
-    <t>JFK</t>
-  </si>
-  <si>
-    <t>KUL</t>
-  </si>
-  <si>
-    <t>MAD</t>
-  </si>
-  <si>
-    <t>SFO</t>
-  </si>
-  <si>
-    <t>CTU</t>
-  </si>
-  <si>
-    <t>BCN</t>
-  </si>
-  <si>
-    <t>BOM</t>
-  </si>
-  <si>
-    <t>SEA</t>
-  </si>
-  <si>
-    <t>LAS</t>
-  </si>
-  <si>
-    <t>Hartsfield-Jackson Atlanta International Airport</t>
-  </si>
-  <si>
-    <t>Beijing Capital International Airport</t>
-  </si>
-  <si>
-    <t>Dubai International Airport</t>
-  </si>
-  <si>
-    <t>Los Angeles International Airport</t>
-  </si>
-  <si>
-    <t>Tokyo Haneda International Airport</t>
-  </si>
-  <si>
-    <t>O'Hare International Airport</t>
-  </si>
-  <si>
-    <t>London Heathrow Airport</t>
-  </si>
-  <si>
-    <t>Hong Kong International Airport</t>
-  </si>
-  <si>
-    <t>Shanghai Pudong International Airport</t>
-  </si>
-  <si>
-    <t>Aéroport Paris-Charles de Gaulle</t>
-  </si>
-  <si>
-    <t>Amsterdam Airport Schiphol</t>
-  </si>
-  <si>
-    <t>Indira Gandhi International Airport</t>
-  </si>
-  <si>
-    <t>Guangzhou Baiyun International Airport</t>
-  </si>
-  <si>
-    <t>Flughafen Frankfurt am Main</t>
-  </si>
-  <si>
-    <t>Dallas/Fort Worth International Airport</t>
-  </si>
-  <si>
-    <t>Seoul Incheon International Airport</t>
-  </si>
-  <si>
-    <t>Istanbul Atatürk Airport</t>
-  </si>
-  <si>
-    <t>Soekarno-Hatta International Airport</t>
-  </si>
-  <si>
-    <t>Singapore Changi Airport</t>
-  </si>
-  <si>
-    <t>Denver International Airport</t>
-  </si>
-  <si>
-    <t>Suvarnabhumi Airport</t>
-  </si>
-  <si>
-    <t>John F. Kennedy International Airport</t>
-  </si>
-  <si>
-    <t>Kuala Lumpur International Airport</t>
-  </si>
-  <si>
-    <t>Aeropuerto de Madrid Barajas</t>
-  </si>
-  <si>
-    <t>San Francisco International Airport</t>
-  </si>
-  <si>
-    <t>Chengdu Shuangliu International Airport</t>
-  </si>
-  <si>
-    <t>Aeroport de Barcelona - el Prat</t>
-  </si>
-  <si>
-    <t>Chhatrapati Shivaji International Airport</t>
-  </si>
-  <si>
-    <t>Seattle-Tacoma International Airport</t>
-  </si>
-  <si>
-    <t>McCarran International Airport</t>
   </si>
 </sst>
 </file>
@@ -522,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,7 +484,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -552,7 +492,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -560,7 +500,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -568,218 +508,138 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>52</v>
-      </c>
-      <c r="B22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>53</v>
-      </c>
-      <c r="B23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>54</v>
-      </c>
-      <c r="B24" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>55</v>
-      </c>
-      <c r="B25" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>56</v>
-      </c>
-      <c r="B26" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>57</v>
-      </c>
-      <c r="B27" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>58</v>
-      </c>
-      <c r="B28" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>59</v>
-      </c>
-      <c r="B29" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>60</v>
-      </c>
-      <c r="B30" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>61</v>
-      </c>
-      <c r="B31" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>